<commit_message>
Bugs corrigidos e adicionadas funcionalidades
</commit_message>
<xml_diff>
--- a/tags_to_change.xlsx
+++ b/tags_to_change.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\replace_dwg_tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99781407-5D2F-489A-9285-1205D5E7AC1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33916B3E-81AD-47FE-AE2F-BBD4C0CC6E16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>2174XAHH101A</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Tt</t>
+  </si>
+  <si>
+    <t>blabla</t>
+  </si>
+  <si>
+    <t>vai dar erro</t>
   </si>
 </sst>
 </file>
@@ -718,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E84F42-CA81-4B96-8F22-E70068506351}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,6 +1189,20 @@
         <v>64</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="2">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>